<commit_message>
Thêm thông tin khách hàng.
</commit_message>
<xml_diff>
--- a/data/processed/customer_credit_data_clean.xlsx
+++ b/data/processed/customer_credit_data_clean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>job</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>main_salary</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>passive_salary</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>credit_score</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>loan_amount</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>debt_to_income</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>repayment_period</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>bank_rate</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>total_income</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>emi</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>dti</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>loan_to_income</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>risk_level</t>
         </is>
       </c>
     </row>
@@ -467,14 +517,48 @@
       <c r="B2" t="n">
         <v>25</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Engineer</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>50000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F2" t="n">
         <v>700</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>10000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>865.2674609813781</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.573213565420687</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -484,14 +568,48 @@
       <c r="B3" t="n">
         <v>40</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Doctor</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>80000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F3" t="n">
         <v>650</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>20000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I3" t="n">
+        <v>24</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>82000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>890.9250286702262</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.086493937402715</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.2439024390243902</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -501,14 +619,48 @@
       <c r="B4" t="n">
         <v>35</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>60000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F4" t="n">
         <v>720</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>15000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I4" t="n">
+        <v>18</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>63000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>883.6857832149394</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.40267584637292</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -518,14 +670,354 @@
       <c r="B5" t="n">
         <v>50</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Artist</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>90000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F5" t="n">
         <v>600</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>25000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>36</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="n">
+        <v>91000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>783.4091365357781</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.8608891610283276</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.2747252747252747</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>29</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>55000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>750</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="I6" t="n">
+        <v>24</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>59000</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1332.32352923643</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.258175473282085</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5084745762711864</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>45</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Nurse</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>65000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>680</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="n">
+        <v>70000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>801.5019594760035</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.145002799251434</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.3142857142857143</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>39</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>70000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4500</v>
+      </c>
+      <c r="F8" t="n">
+        <v>710</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>24</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>74500</v>
+      </c>
+      <c r="L8" t="n">
+        <v>804.275382516881</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.07956427183474</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.2416107382550336</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>55</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Lawyer</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>95000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>640</v>
+      </c>
+      <c r="G9" t="n">
+        <v>20000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="I9" t="n">
+        <v>36</v>
+      </c>
+      <c r="J9" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>97000</v>
+      </c>
+      <c r="L9" t="n">
+        <v>619.3724435719324</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.6385282923421984</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2061855670103093</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>28</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Chef</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>70000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>650</v>
+      </c>
+      <c r="G10" t="n">
+        <v>35000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I10" t="n">
+        <v>36</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>76000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1072.71510067785</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.411467237734013</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.4605263157894737</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>60</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>120000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>720</v>
+      </c>
+      <c r="G11" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I11" t="n">
+        <v>48</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>127000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1208.945096886547</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.9519252731390131</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.3937007874015748</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>